<commit_message>
Ajuste na frases de Bandido
</commit_message>
<xml_diff>
--- a/Release 1/_resources/Combinações.xlsx
+++ b/Release 1/_resources/Combinações.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="4275" yWindow="0" windowWidth="19065" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="5700" yWindow="0" windowWidth="19065" windowHeight="8940" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Negócios" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
   <si>
     <t>das formas de ação.</t>
   </si>
@@ -355,9 +355,6 @@
     <t>é caso perdido pra você</t>
   </si>
   <si>
-    <t>não é mais teu</t>
-  </si>
-  <si>
     <t>BANDIDO</t>
   </si>
   <si>
@@ -389,6 +386,12 @@
   </si>
   <si>
     <t>e tu fica livre da cidade do pé junto.</t>
+  </si>
+  <si>
+    <t>não é mais</t>
+  </si>
+  <si>
+    <t>a bike</t>
   </si>
 </sst>
 </file>
@@ -1511,7 +1514,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1541,7 +1546,7 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>81</v>
@@ -1553,7 +1558,7 @@
         <v>99</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>"'" &amp; B2 &amp; "',"</f>
@@ -1584,7 +1589,7 @@
         <v>100</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G3" s="7" t="str">
         <f t="shared" ref="G3:J11" si="0">"'" &amp; B3 &amp; "',"</f>
@@ -1615,7 +1620,7 @@
         <v>101</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1646,7 +1651,7 @@
         <v>102</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="G5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1677,7 +1682,7 @@
         <v>103</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1708,7 +1713,7 @@
         <v>105</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1739,7 +1744,7 @@
         <v>106</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1770,7 +1775,7 @@
         <v>107</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="G9" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1801,7 +1806,7 @@
         <v>108</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1826,13 +1831,13 @@
         <v>95</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>91</v>
+        <v>121</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>109</v>
+        <v>120</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1840,11 +1845,11 @@
       </c>
       <c r="H11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'a carteira',</v>
+        <v>'a bike',</v>
       </c>
       <c r="I11" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'não é mais teu',</v>
+        <v>'não é mais',</v>
       </c>
       <c r="J11" s="7" t="str">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Assunto Vitima do Bandido.
</commit_message>
<xml_diff>
--- a/Release 1/_resources/Combinações.xlsx
+++ b/Release 1/_resources/Combinações.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="0" windowWidth="19065" windowHeight="8940" activeTab="2"/>
+    <workbookView xWindow="8550" yWindow="0" windowWidth="19065" windowHeight="8940" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Negócios" sheetId="1" r:id="rId1"/>
     <sheet name="Informática" sheetId="2" r:id="rId2"/>
     <sheet name="Bandido" sheetId="3" r:id="rId3"/>
+    <sheet name="Vítima" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="155">
   <si>
     <t>das formas de ação.</t>
   </si>
@@ -325,15 +326,9 @@
     <t>a mochila</t>
   </si>
   <si>
-    <t>já não é seu</t>
-  </si>
-  <si>
     <t>tu vai passar</t>
   </si>
   <si>
-    <t>tu larga e vai embora</t>
-  </si>
-  <si>
     <t>vai ficar com a parceria aqui</t>
   </si>
   <si>
@@ -358,27 +353,18 @@
     <t>BANDIDO</t>
   </si>
   <si>
-    <t>e vai andando sem olhar pra trás.</t>
-  </si>
-  <si>
     <t>e se gritar tu perde mais.</t>
   </si>
   <si>
     <t>pra tu largar de ser otário.</t>
   </si>
   <si>
-    <t>e vai saindo no sapatinho.</t>
-  </si>
-  <si>
     <t>pra tu ficar sabendo quem manda no pedaço.</t>
   </si>
   <si>
     <t>pra tu sai na boa daqui.</t>
   </si>
   <si>
-    <t>e tu não leva uma azeitona.</t>
-  </si>
-  <si>
     <t>pra barra ficar leve pra tu.</t>
   </si>
   <si>
@@ -392,6 +378,120 @@
   </si>
   <si>
     <t>a bike</t>
+  </si>
+  <si>
+    <t>tu vai largar e vai embora</t>
+  </si>
+  <si>
+    <t>já não é coisa tua</t>
+  </si>
+  <si>
+    <t>e agora vai andando sem olhar pra trás.</t>
+  </si>
+  <si>
+    <t>e agora tu vai saindo no sapatinho.</t>
+  </si>
+  <si>
+    <t>só pra tu não levar um sacode.</t>
+  </si>
+  <si>
+    <t>Por favor, moço,</t>
+  </si>
+  <si>
+    <t>Faz isso comigo não,</t>
+  </si>
+  <si>
+    <t>Calma, calma,</t>
+  </si>
+  <si>
+    <t>Ai, meu Deus do céu,</t>
+  </si>
+  <si>
+    <t>Logo eu,</t>
+  </si>
+  <si>
+    <t>Pode levar tudo, mas me deixa vivo,</t>
+  </si>
+  <si>
+    <t>Eu já fui assaltado hoje, moço,</t>
+  </si>
+  <si>
+    <t>Pode pegar, eu não vou resistir, mas</t>
+  </si>
+  <si>
+    <t>É seu, perdi, mas</t>
+  </si>
+  <si>
+    <t>eu não quero,</t>
+  </si>
+  <si>
+    <t>vocês levam,</t>
+  </si>
+  <si>
+    <t>eu não ligo, pode levar,</t>
+  </si>
+  <si>
+    <t>é de vocês,</t>
+  </si>
+  <si>
+    <t>outra vez? Tudo bem, leva,</t>
+  </si>
+  <si>
+    <t>VÍTIMA</t>
+  </si>
+  <si>
+    <t>Fica tranquilo, já</t>
+  </si>
+  <si>
+    <t>é emprestado, por favor,</t>
+  </si>
+  <si>
+    <t>não, tem piedade, moço</t>
+  </si>
+  <si>
+    <t>nem paguei ainda</t>
+  </si>
+  <si>
+    <t>o anel</t>
+  </si>
+  <si>
+    <t>o iPhone</t>
+  </si>
+  <si>
+    <t>mas me deixa ir, moço.</t>
+  </si>
+  <si>
+    <t>e pode levar o que quiser.</t>
+  </si>
+  <si>
+    <t>e não vou reagir, fica calmo, moço.</t>
+  </si>
+  <si>
+    <t>mas não me machuca.</t>
+  </si>
+  <si>
+    <t>mas por favor, moço, me deixa sair.</t>
+  </si>
+  <si>
+    <t>eu preciso muito, é de família, leva o dinheiro</t>
+  </si>
+  <si>
+    <t>não, toma minha carteira,</t>
+  </si>
+  <si>
+    <t>mas me deixa sair vivo.</t>
+  </si>
+  <si>
+    <t>mas tem misericórdia, por favor, me deixa sair.</t>
+  </si>
+  <si>
+    <t>me deixar ir.</t>
+  </si>
+  <si>
+    <t>eu vou ficar parado, não vou reagir.</t>
+  </si>
+  <si>
+    <t>me deixa em paz, não me bate.</t>
   </si>
 </sst>
 </file>
@@ -1514,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2:J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1546,7 +1646,7 @@
     </row>
     <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>81</v>
@@ -1555,10 +1655,10 @@
         <v>89</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="G2" s="7" t="str">
         <f>"'" &amp; B2 &amp; "',"</f>
@@ -1570,7 +1670,7 @@
       </c>
       <c r="I2" s="7" t="str">
         <f>"'" &amp; D2 &amp; "',"</f>
-        <v>'já não é seu',</v>
+        <v>'já não é coisa tua',</v>
       </c>
       <c r="J2" s="7" t="str">
         <f>"'" &amp; E2 &amp; "',"</f>
@@ -1586,10 +1686,10 @@
         <v>90</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="G3" s="7" t="str">
         <f t="shared" ref="G3:J11" si="0">"'" &amp; B3 &amp; "',"</f>
@@ -1617,10 +1717,10 @@
         <v>91</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>101</v>
+        <v>117</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
       <c r="G4" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1632,11 +1732,11 @@
       </c>
       <c r="I4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'tu larga e vai embora',</v>
+        <v>'tu vai largar e vai embora',</v>
       </c>
       <c r="J4" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'e vai andando sem olhar pra trás.',</v>
+        <v>'e agora vai andando sem olhar pra trás.',</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1648,10 +1748,10 @@
         <v>92</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
       <c r="G5" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1667,7 +1767,7 @@
       </c>
       <c r="J5" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'e vai saindo no sapatinho.',</v>
+        <v>'só pra tu não levar um sacode.',</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
@@ -1679,10 +1779,10 @@
         <v>93</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G6" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1710,10 +1810,10 @@
         <v>94</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G7" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1741,10 +1841,10 @@
         <v>96</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="G8" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1760,7 +1860,7 @@
       </c>
       <c r="J8" s="7" t="str">
         <f t="shared" si="0"/>
-        <v>'e tu não leva uma azeitona.',</v>
+        <v>'e agora tu vai saindo no sapatinho.',</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1772,10 +1872,10 @@
         <v>97</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="G9" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1797,16 +1897,16 @@
     <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A10" s="8"/>
       <c r="B10" s="4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C10" s="4" t="s">
         <v>98</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G10" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1831,13 +1931,13 @@
         <v>95</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="G11" s="7" t="str">
         <f t="shared" si="0"/>
@@ -1854,6 +1954,359 @@
       <c r="J11" s="7" t="str">
         <f t="shared" si="0"/>
         <v>'e tu fica livre da cidade do pé junto.',</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:A11"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScalePageLayoutView="85" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="5.5703125" style="1" customWidth="1"/>
+    <col min="2" max="3" width="21" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21" style="6" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="1"/>
+    <col min="7" max="10" width="8.28515625" style="7" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="2"/>
+      <c r="B1" s="3">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1" s="3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="G2" s="7" t="str">
+        <f>"'" &amp; B2 &amp; "',"</f>
+        <v>'Por favor, moço,',</v>
+      </c>
+      <c r="H2" s="7" t="str">
+        <f>"'" &amp; C2 &amp; "',"</f>
+        <v>'o celular',</v>
+      </c>
+      <c r="I2" s="7" t="str">
+        <f>"'" &amp; D2 &amp; "',"</f>
+        <v>'não, toma minha carteira,',</v>
+      </c>
+      <c r="J2" s="7" t="str">
+        <f>"'" &amp; E2 &amp; "',"</f>
+        <v>'mas me deixa ir, moço.',</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
+      <c r="B3" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>134</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="G3" s="7" t="str">
+        <f t="shared" ref="G3:J11" si="0">"'" &amp; B3 &amp; "',"</f>
+        <v>'Faz isso comigo não,',</v>
+      </c>
+      <c r="H3" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o relógio',</v>
+      </c>
+      <c r="I3" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'é de vocês,',</v>
+      </c>
+      <c r="J3" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'e pode levar o que quiser.',</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="8"/>
+      <c r="B4" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="G4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Calma, calma,',</v>
+      </c>
+      <c r="H4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o iPhone',</v>
+      </c>
+      <c r="I4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'eu não ligo, pode levar,',</v>
+      </c>
+      <c r="J4" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'e não vou reagir, fica calmo, moço.',</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
+      <c r="B5" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Fica tranquilo, já',</v>
+      </c>
+      <c r="H5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o tênis',</v>
+      </c>
+      <c r="I5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'eu não quero,',</v>
+      </c>
+      <c r="J5" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'mas não me machuca.',</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>132</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="G6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Ai, meu Deus do céu,',</v>
+      </c>
+      <c r="H6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o carro',</v>
+      </c>
+      <c r="I6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'vocês levam,',</v>
+      </c>
+      <c r="J6" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'mas por favor, moço, me deixa sair.',</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
+      <c r="B7" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="G7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Logo eu,',</v>
+      </c>
+      <c r="H7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'a moto',</v>
+      </c>
+      <c r="I7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'outra vez? Tudo bem, leva,',</v>
+      </c>
+      <c r="J7" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'mas me deixa sair vivo.',</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
+      <c r="B8" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="G8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Eu já fui assaltado hoje, moço,',</v>
+      </c>
+      <c r="H8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o anel',</v>
+      </c>
+      <c r="I8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'eu preciso muito, é de família, leva o dinheiro',</v>
+      </c>
+      <c r="J8" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'mas tem misericórdia, por favor, me deixa sair.',</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>152</v>
+      </c>
+      <c r="G9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Pode levar tudo, mas me deixa vivo,',</v>
+      </c>
+      <c r="H9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'o cordão',</v>
+      </c>
+      <c r="I9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'é emprestado, por favor,',</v>
+      </c>
+      <c r="J9" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'me deixar ir.',</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="8"/>
+      <c r="B10" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>153</v>
+      </c>
+      <c r="G10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'Pode pegar, eu não vou resistir, mas',</v>
+      </c>
+      <c r="H10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'a mochila',</v>
+      </c>
+      <c r="I10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'não, tem piedade, moço',</v>
+      </c>
+      <c r="J10" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'eu vou ficar parado, não vou reagir.',</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="8"/>
+      <c r="B11" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="G11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'É seu, perdi, mas',</v>
+      </c>
+      <c r="H11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'a bike',</v>
+      </c>
+      <c r="I11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'nem paguei ainda',</v>
+      </c>
+      <c r="J11" s="7" t="str">
+        <f t="shared" si="0"/>
+        <v>'me deixa em paz, não me bate.',</v>
       </c>
     </row>
   </sheetData>

</xml_diff>